<commit_message>
Added Provincial BLGF data
</commit_message>
<xml_diff>
--- a/PSA-Poverty-Data.xlsx
+++ b/PSA-Poverty-Data.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R Projects\PH-LGU-Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{600E8E2A-AE73-4E0D-8F39-DB041CDEF990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{863B64B0-1687-473A-81F8-223790679FC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="405" yWindow="3870" windowWidth="14385" windowHeight="10500" xr2:uid="{0B391317-C9C8-4981-B78B-63E495DFDBBB}"/>
+    <workbookView xWindow="4755" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{0B391317-C9C8-4981-B78B-63E495DFDBBB}"/>
   </bookViews>
   <sheets>
     <sheet name="2009-2015" sheetId="1" r:id="rId1"/>
+    <sheet name="metadata" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6556" uniqueCount="3141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6608" uniqueCount="3152">
   <si>
     <t>PSGC</t>
   </si>
@@ -9457,13 +9458,46 @@
   </si>
   <si>
     <t>157011000</t>
+  </si>
+  <si>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Data Type</t>
+  </si>
+  <si>
+    <t>Unit of Measurement</t>
+  </si>
+  <si>
+    <t>PSA - PSGC, as of 2020 Q4</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>Decimal</t>
+  </si>
+  <si>
+    <t>PSA - 2009 Poverty Statistics</t>
+  </si>
+  <si>
+    <t>PSA - 2012 Poverty Statistics</t>
+  </si>
+  <si>
+    <t>PSA - 2015 Poverty Statistics</t>
+  </si>
+  <si>
+    <t>percent</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -9473,6 +9507,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -9498,7 +9540,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -9509,6 +9551,18 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -9830,7 +9884,7 @@
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -77291,4 +77345,210 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A27E03F-EB3B-4697-A9A6-F6622EFE4DF0}">
+  <dimension ref="A1:D14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.5703125" customWidth="1"/>
+    <col min="2" max="2" width="42.85546875" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" customWidth="1"/>
+    <col min="4" max="4" width="28.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>3141</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>3142</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>3143</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>3144</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3145</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3146</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3145</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3146</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3145</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3146</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3145</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3146</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3148</v>
+      </c>
+      <c r="C6" t="s">
+        <v>3147</v>
+      </c>
+      <c r="D6" t="s">
+        <v>3151</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3149</v>
+      </c>
+      <c r="C7" t="s">
+        <v>3147</v>
+      </c>
+      <c r="D7" t="s">
+        <v>3151</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3150</v>
+      </c>
+      <c r="C8" t="s">
+        <v>3147</v>
+      </c>
+      <c r="D8" t="s">
+        <v>3151</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3148</v>
+      </c>
+      <c r="C9" t="s">
+        <v>3147</v>
+      </c>
+      <c r="D9" t="s">
+        <v>3151</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="B10" t="s">
+        <v>3148</v>
+      </c>
+      <c r="C10" t="s">
+        <v>3147</v>
+      </c>
+      <c r="D10" t="s">
+        <v>3151</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3149</v>
+      </c>
+      <c r="C11" t="s">
+        <v>3147</v>
+      </c>
+      <c r="D11" t="s">
+        <v>3151</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="B12" t="s">
+        <v>3149</v>
+      </c>
+      <c r="C12" t="s">
+        <v>3147</v>
+      </c>
+      <c r="D12" t="s">
+        <v>3151</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="B13" t="s">
+        <v>3150</v>
+      </c>
+      <c r="C13" t="s">
+        <v>3147</v>
+      </c>
+      <c r="D13" t="s">
+        <v>3151</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="B14" t="s">
+        <v>3150</v>
+      </c>
+      <c r="C14" t="s">
+        <v>3147</v>
+      </c>
+      <c r="D14" t="s">
+        <v>3151</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>